<commit_message>
Update spreadsheet, fix profile name in constraint
</commit_message>
<xml_diff>
--- a/requirements/Anonymized eicrdataneedsv14_working.xlsx
+++ b/requirements/Anonymized eicrdataneedsv14_working.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\Lantana\FHIR-us-eicr-anonymized\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0136AB89-428B-457A-828E-25EC2DBD11A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F84C38-B7D3-410C-AC97-B1C6A562262E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{285485E5-942A-4B88-BF4B-14F3EF0BB33E}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="599">
   <si>
     <t>eICR Data Element</t>
   </si>
@@ -1893,6 +1893,15 @@
   </si>
   <si>
     <t>Disallow slice, template</t>
+  </si>
+  <si>
+    <t>All relevent data elements</t>
+  </si>
+  <si>
+    <t>*.display</t>
+  </si>
+  <si>
+    <t>Disallow display on all relevant data elements</t>
   </si>
 </sst>
 </file>
@@ -2428,9 +2437,9 @@
   <dimension ref="A1:M228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8599,8 +8608,30 @@
         <v>484</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B201" s="13"/>
+    <row r="201" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+      <c r="A201" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="B201" s="20"/>
+      <c r="C201" s="19"/>
+      <c r="D201" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="E201" s="11"/>
+      <c r="F201" s="7"/>
+      <c r="G201" s="7"/>
+      <c r="H201" s="7"/>
+      <c r="I201" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="J201" s="11"/>
+      <c r="K201" s="11"/>
+      <c r="L201" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="M201" s="11" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B202" s="13"/>
@@ -9453,32 +9484,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ed5a28f-e285-4793-933e-f86572ea3e88" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAEF04E9A1B48544A813770D804417BF" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a681fcb199cf8f7d334bb0be32bb6121">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="910aa554c65bba8b8ae3e351c6d836ba" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9761,10 +9766,50 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ed5a28f-e285-4793-933e-f86572ea3e88" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0EC9102-CC0B-48A4-9231-EA87BE55FEC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
+    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
+    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
+    <ds:schemaRef ds:uri="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9790,23 +9835,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0EC9102-CC0B-48A4-9231-EA87BE55FEC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
-    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
-    <ds:schemaRef ds:uri="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Prescribe MASKED text.div in Past Medical History section and History of Present Illness (constraint)
</commit_message>
<xml_diff>
--- a/requirements/Anonymized eicrdataneedsv14_working.xlsx
+++ b/requirements/Anonymized eicrdataneedsv14_working.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\Lantana\FHIR-us-eicr-anonymized\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F84C38-B7D3-410C-AC97-B1C6A562262E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CAD8D7-0DDB-49FA-82E8-5D2B76B8FA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{285485E5-942A-4B88-BF4B-14F3EF0BB33E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{285485E5-942A-4B88-BF4B-14F3EF0BB33E}"/>
   </bookViews>
   <sheets>
     <sheet name="eICR Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'data elements'!$A$1:$K$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'eICR Data'!$A$1:$I$200</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'eICR Data'!$A$1:$I$201</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1889,9 +1889,6 @@
     <t>eICR Composition.socialHistorySection.ExposureContactInformation</t>
   </si>
   <si>
-    <t>disallow text in section</t>
-  </si>
-  <si>
     <t>Disallow slice, template</t>
   </si>
   <si>
@@ -1902,6 +1899,9 @@
   </si>
   <si>
     <t>Disallow display on all relevant data elements</t>
+  </si>
+  <si>
+    <t>prescribe MASKED text in section.text.div (had to use a constraint for this because the xHtml data type doesn't allow fixing a value)</t>
   </si>
 </sst>
 </file>
@@ -2434,12 +2434,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0C505-63DE-4322-BEE9-180C5089B356}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M228"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="D201" sqref="D201"/>
+      <selection pane="bottomLeft" activeCell="L198" sqref="L198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2499,7 +2500,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>448</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>448</v>
       </c>
@@ -2561,7 +2562,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>448</v>
       </c>
@@ -2590,7 +2591,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>448</v>
       </c>
@@ -2917,7 +2918,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>462</v>
       </c>
@@ -2954,7 +2955,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>463</v>
       </c>
@@ -2993,7 +2994,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>448</v>
       </c>
@@ -3024,7 +3025,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>448</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>448</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>448</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>448</v>
       </c>
@@ -3150,7 +3151,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>448</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>448</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>448</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>448</v>
       </c>
@@ -3276,7 +3277,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>448</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>448</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>448</v>
       </c>
@@ -3365,7 +3366,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>448</v>
       </c>
@@ -3394,7 +3395,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>448</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="1" customFormat="1" ht="96" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>448</v>
       </c>
@@ -3643,7 +3644,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>448</v>
       </c>
@@ -3674,7 +3675,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" s="1" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>448</v>
       </c>
@@ -3711,7 +3712,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>448</v>
       </c>
@@ -3816,7 +3817,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>448</v>
       </c>
@@ -3851,7 +3852,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>448</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>448</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>448</v>
       </c>
@@ -3944,7 +3945,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>448</v>
       </c>
@@ -3977,7 +3978,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>448</v>
       </c>
@@ -4010,7 +4011,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>448</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>448</v>
       </c>
@@ -4111,7 +4112,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>448</v>
       </c>
@@ -4140,7 +4141,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>448</v>
       </c>
@@ -4169,7 +4170,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>448</v>
       </c>
@@ -4198,7 +4199,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>448</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>448</v>
       </c>
@@ -4258,7 +4259,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>448</v>
       </c>
@@ -4289,7 +4290,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>448</v>
       </c>
@@ -4320,7 +4321,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>448</v>
       </c>
@@ -4349,7 +4350,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>448</v>
       </c>
@@ -4380,7 +4381,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>448</v>
       </c>
@@ -4409,7 +4410,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>448</v>
       </c>
@@ -4440,7 +4441,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>448</v>
       </c>
@@ -4469,7 +4470,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>448</v>
       </c>
@@ -4500,7 +4501,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>448</v>
       </c>
@@ -4529,7 +4530,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>448</v>
       </c>
@@ -4560,7 +4561,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>448</v>
       </c>
@@ -4591,7 +4592,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>448</v>
       </c>
@@ -4624,7 +4625,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>448</v>
       </c>
@@ -4657,7 +4658,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="68" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>445</v>
       </c>
@@ -4686,13 +4687,13 @@
       </c>
       <c r="K68" s="4"/>
       <c r="L68" s="7" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="M68" s="4" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="69" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>448</v>
       </c>
@@ -4723,7 +4724,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="70" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>448</v>
       </c>
@@ -4754,7 +4755,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="71" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>448</v>
       </c>
@@ -4785,7 +4786,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="72" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>448</v>
       </c>
@@ -4816,7 +4817,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="73" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>448</v>
       </c>
@@ -4849,7 +4850,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="74" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>448</v>
       </c>
@@ -4880,7 +4881,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="75" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>448</v>
       </c>
@@ -4911,7 +4912,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="76" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>448</v>
       </c>
@@ -4944,7 +4945,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="77" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>448</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="78" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>448</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>448</v>
       </c>
@@ -5039,7 +5040,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>448</v>
       </c>
@@ -5070,7 +5071,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="81" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>448</v>
       </c>
@@ -5099,7 +5100,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>448</v>
       </c>
@@ -5130,7 +5131,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>448</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="84" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>448</v>
       </c>
@@ -5190,7 +5191,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>448</v>
       </c>
@@ -5219,7 +5220,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="86" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>448</v>
       </c>
@@ -5248,7 +5249,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="87" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>448</v>
       </c>
@@ -5277,7 +5278,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>448</v>
       </c>
@@ -5308,7 +5309,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>448</v>
       </c>
@@ -5337,7 +5338,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="90" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>448</v>
       </c>
@@ -5368,7 +5369,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>448</v>
       </c>
@@ -5399,7 +5400,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>448</v>
       </c>
@@ -5430,7 +5431,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>448</v>
       </c>
@@ -5461,7 +5462,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="94" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>448</v>
       </c>
@@ -5492,7 +5493,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="95" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>448</v>
       </c>
@@ -5525,7 +5526,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>448</v>
       </c>
@@ -5556,7 +5557,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="97" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>448</v>
       </c>
@@ -5587,7 +5588,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="98" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>448</v>
       </c>
@@ -5618,7 +5619,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="99" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>448</v>
       </c>
@@ -5649,7 +5650,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="100" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>448</v>
       </c>
@@ -5680,7 +5681,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="101" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>448</v>
       </c>
@@ -5711,7 +5712,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="102" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>448</v>
       </c>
@@ -5742,7 +5743,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="103" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="23" t="s">
         <v>448</v>
       </c>
@@ -5773,7 +5774,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="104" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" s="1" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="23" t="s">
         <v>448</v>
       </c>
@@ -5804,7 +5805,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="105" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>448</v>
       </c>
@@ -5835,7 +5836,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="106" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>448</v>
       </c>
@@ -5866,7 +5867,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="107" spans="1:13" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" s="1" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>448</v>
       </c>
@@ -5899,7 +5900,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="108" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>448</v>
       </c>
@@ -5932,7 +5933,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="109" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>448</v>
       </c>
@@ -5963,7 +5964,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>448</v>
       </c>
@@ -5992,7 +5993,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>448</v>
       </c>
@@ -6021,7 +6022,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>448</v>
       </c>
@@ -6050,7 +6051,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>448</v>
       </c>
@@ -6079,7 +6080,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>448</v>
       </c>
@@ -6108,7 +6109,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>448</v>
       </c>
@@ -6137,7 +6138,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>448</v>
       </c>
@@ -6166,7 +6167,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>448</v>
       </c>
@@ -6195,7 +6196,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>448</v>
       </c>
@@ -6224,7 +6225,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>448</v>
       </c>
@@ -6253,7 +6254,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>448</v>
       </c>
@@ -6282,7 +6283,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>448</v>
       </c>
@@ -6311,7 +6312,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>448</v>
       </c>
@@ -6340,7 +6341,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>448</v>
       </c>
@@ -6369,7 +6370,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>448</v>
       </c>
@@ -6398,7 +6399,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>448</v>
       </c>
@@ -6427,7 +6428,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>448</v>
       </c>
@@ -6456,7 +6457,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>448</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>448</v>
       </c>
@@ -6514,7 +6515,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>448</v>
       </c>
@@ -6543,7 +6544,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>448</v>
       </c>
@@ -6572,7 +6573,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>448</v>
       </c>
@@ -6599,7 +6600,7 @@
       <c r="L131" s="11"/>
       <c r="M131" s="11"/>
     </row>
-    <row r="132" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>448</v>
       </c>
@@ -6628,7 +6629,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>448</v>
       </c>
@@ -6657,7 +6658,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="134" spans="1:13" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" s="1" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>448</v>
       </c>
@@ -6686,7 +6687,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="135" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>448</v>
       </c>
@@ -6715,7 +6716,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="136" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>448</v>
       </c>
@@ -6744,7 +6745,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="137" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>448</v>
       </c>
@@ -6773,7 +6774,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="138" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>448</v>
       </c>
@@ -6802,7 +6803,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="139" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>448</v>
       </c>
@@ -6866,7 +6867,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="141" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23" t="s">
         <v>448</v>
       </c>
@@ -6895,7 +6896,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="142" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="23" t="s">
         <v>448</v>
       </c>
@@ -6924,7 +6925,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="143" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>448</v>
       </c>
@@ -6953,7 +6954,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="144" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" s="1" customFormat="1" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>448</v>
       </c>
@@ -6982,7 +6983,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="145" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>448</v>
       </c>
@@ -7011,7 +7012,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="146" spans="1:13" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" s="1" customFormat="1" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>448</v>
       </c>
@@ -7040,7 +7041,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>448</v>
       </c>
@@ -7069,7 +7070,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>448</v>
       </c>
@@ -7098,7 +7099,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="72" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" ht="72" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>448</v>
       </c>
@@ -7127,7 +7128,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" ht="84" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="23" t="s">
         <v>448</v>
       </c>
@@ -7156,7 +7157,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="23" t="s">
         <v>448</v>
       </c>
@@ -7185,7 +7186,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="23" t="s">
         <v>448</v>
       </c>
@@ -7214,7 +7215,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="23" t="s">
         <v>448</v>
       </c>
@@ -7243,7 +7244,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="84" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" ht="84" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>448</v>
       </c>
@@ -7377,7 +7378,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="158" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
         <v>448</v>
       </c>
@@ -7406,7 +7407,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="11" t="s">
         <v>448</v>
       </c>
@@ -7435,7 +7436,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="160" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="11" t="s">
         <v>448</v>
       </c>
@@ -7464,7 +7465,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="161" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
         <v>445</v>
       </c>
@@ -7491,13 +7492,13 @@
       </c>
       <c r="K161" s="11"/>
       <c r="L161" s="7" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="M161" s="11" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="11" t="s">
         <v>448</v>
       </c>
@@ -7524,7 +7525,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="163" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
         <v>448</v>
       </c>
@@ -7553,7 +7554,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="164" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
         <v>448</v>
       </c>
@@ -7582,7 +7583,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="165" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
         <v>448</v>
       </c>
@@ -7611,7 +7612,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
         <v>448</v>
       </c>
@@ -7640,7 +7641,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="167" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="11" t="s">
         <v>448</v>
       </c>
@@ -7671,7 +7672,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="11" t="s">
         <v>448</v>
       </c>
@@ -7700,7 +7701,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="36" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" ht="36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="11" t="s">
         <v>448</v>
       </c>
@@ -7729,7 +7730,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="20" t="s">
         <v>448</v>
       </c>
@@ -7760,7 +7761,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="171" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="20" t="s">
         <v>448</v>
       </c>
@@ -7791,7 +7792,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="20" t="s">
         <v>448</v>
       </c>
@@ -7822,7 +7823,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="20" t="s">
         <v>448</v>
       </c>
@@ -7853,7 +7854,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="20" t="s">
         <v>448</v>
       </c>
@@ -7884,7 +7885,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="20" t="s">
         <v>448</v>
       </c>
@@ -7915,7 +7916,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="176" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="20" t="s">
         <v>448</v>
       </c>
@@ -7944,7 +7945,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="177" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="20" t="s">
         <v>448</v>
       </c>
@@ -7975,7 +7976,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="178" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="20" t="s">
         <v>448</v>
       </c>
@@ -8006,7 +8007,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="179" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="20" t="s">
         <v>448</v>
       </c>
@@ -8037,7 +8038,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="180" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="20" t="s">
         <v>448</v>
       </c>
@@ -8068,7 +8069,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="181" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="20" t="s">
         <v>448</v>
       </c>
@@ -8099,7 +8100,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="182" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="20" t="s">
         <v>448</v>
       </c>
@@ -8128,7 +8129,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="183" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
         <v>448</v>
       </c>
@@ -8186,13 +8187,13 @@
       </c>
       <c r="K184" s="11"/>
       <c r="L184" s="7" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="M184" s="4" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="185" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="11" t="s">
         <v>448</v>
       </c>
@@ -8221,7 +8222,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="11" t="s">
         <v>448</v>
       </c>
@@ -8250,7 +8251,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="187" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
         <v>448</v>
       </c>
@@ -8279,7 +8280,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="188" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
         <v>448</v>
       </c>
@@ -8308,7 +8309,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="189" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="11" t="s">
         <v>448</v>
       </c>
@@ -8339,7 +8340,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="11" t="s">
         <v>467</v>
       </c>
@@ -8362,7 +8363,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="11" t="s">
         <v>467</v>
       </c>
@@ -8385,7 +8386,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="192" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="11" t="s">
         <v>467</v>
       </c>
@@ -8408,7 +8409,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="193" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" ht="24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="11" t="s">
         <v>467</v>
       </c>
@@ -8431,7 +8432,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="194" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="7" t="s">
         <v>468</v>
       </c>
@@ -8454,7 +8455,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="11" t="s">
         <v>467</v>
       </c>
@@ -8477,7 +8478,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="11" t="s">
         <v>467</v>
       </c>
@@ -8615,19 +8616,19 @@
       <c r="B201" s="20"/>
       <c r="C201" s="19"/>
       <c r="D201" s="11" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E201" s="11"/>
       <c r="F201" s="7"/>
       <c r="G201" s="7"/>
       <c r="H201" s="7"/>
       <c r="I201" s="22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="J201" s="11"/>
       <c r="K201" s="11"/>
       <c r="L201" s="7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M201" s="11" t="s">
         <v>484</v>
@@ -8710,7 +8711,13 @@
       <c r="B228" s="13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I200" xr:uid="{C5F0C505-63DE-4322-BEE9-180C5089B356}"/>
+  <autoFilter ref="A1:I201" xr:uid="{C5F0C505-63DE-4322-BEE9-180C5089B356}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="remove"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
@@ -9484,6 +9491,32 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </LCG_x0020_Document_x0020_Workflow>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9ed5a28f-e285-4793-933e-f86572ea3e88" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AAEF04E9A1B48544A813770D804417BF" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a681fcb199cf8f7d334bb0be32bb6121">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="9ed5a28f-e285-4793-933e-f86572ea3e88" xmlns:ns3="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628" xmlns:ns4="a130c0bc-081d-4a7d-8c4b-0d956631a56e" xmlns:ns5="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="910aa554c65bba8b8ae3e351c6d836ba" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9766,50 +9799,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LCG_x0020_Document_x0020_Workflow xmlns="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </LCG_x0020_Document_x0020_Workflow>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9ed5a28f-e285-4793-933e-f86572ea3e88" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0EC9102-CC0B-48A4-9231-EA87BE55FEC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
-    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
-    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
-    <ds:schemaRef ds:uri="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9835,9 +9828,23 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{444632C0-B354-4144-8906-CF8857243D1F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0EC9102-CC0B-48A4-9231-EA87BE55FEC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="9ed5a28f-e285-4793-933e-f86572ea3e88"/>
+    <ds:schemaRef ds:uri="82D0F40D-97DD-4AB3-B4BB-3ECBE327B628"/>
+    <ds:schemaRef ds:uri="a130c0bc-081d-4a7d-8c4b-0d956631a56e"/>
+    <ds:schemaRef ds:uri="82d0f40d-97dd-4ab3-b4bb-3ecbe327b628"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>